<commit_message>
Cambio de nombre y restructuración de las carpetas de ejecución del mes de Febrero
</commit_message>
<xml_diff>
--- a/Documentos Adicionales/Ventas Adriana Jaramillo.xlsx
+++ b/Documentos Adicionales/Ventas Adriana Jaramillo.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="120" windowWidth="11655" windowHeight="6915"/>
@@ -12,7 +12,7 @@
     <sheet name="ABRIL" sheetId="3" r:id="rId3"/>
     <sheet name="MAYO" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -46,9 +46,6 @@
     <t>EJECUTIVO DE VENTAS:</t>
   </si>
   <si>
-    <t>Alma Yesenia Garcia Enriquez</t>
-  </si>
-  <si>
     <t>META COMISIONABLE:</t>
   </si>
   <si>
@@ -66,17 +63,20 @@
   <si>
     <t>MAYO</t>
   </si>
+  <si>
+    <t>Judith Adriana Jaramillo Chávez</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -363,6 +363,11 @@
       <color rgb="FFFFFF66"/>
     </mruColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -441,6 +446,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -475,6 +481,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -650,37 +657,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="9" max="9" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="26"/>
       <c r="C2" s="27" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D2" s="27"/>
       <c r="E2" s="27"/>
       <c r="G2" s="25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H2" s="26"/>
       <c r="I2" s="28">
         <v>43000</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="18.75">
+    <row r="4" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B4" s="33" t="s">
         <v>7</v>
       </c>
@@ -691,7 +698,7 @@
       <c r="G4" s="33"/>
       <c r="H4" s="33"/>
     </row>
-    <row r="5" spans="1:9" ht="15.75">
+    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
@@ -714,10 +721,10 @@
         <v>6</v>
       </c>
       <c r="I5" s="22" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="4">
         <v>1</v>
       </c>
@@ -741,7 +748,7 @@
       </c>
       <c r="I6" s="23"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="10"/>
       <c r="C7" s="11">
         <v>0</v>
@@ -762,7 +769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="7">
         <v>8</v>
       </c>
@@ -786,7 +793,7 @@
       </c>
       <c r="I8" s="9"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="12">
         <v>825</v>
       </c>
@@ -809,7 +816,7 @@
         <v>3300</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" s="5">
         <v>15</v>
       </c>
@@ -833,7 +840,7 @@
       </c>
       <c r="I10" s="23"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" s="14">
         <v>0</v>
       </c>
@@ -856,7 +863,7 @@
         <v>6915</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" s="7">
         <v>22</v>
       </c>
@@ -880,7 +887,7 @@
       </c>
       <c r="I12" s="23"/>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" s="12">
         <v>825</v>
       </c>
@@ -899,7 +906,7 @@
         <v>1237.5</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" s="5">
         <v>29</v>
       </c>
@@ -911,7 +918,7 @@
       <c r="H14" s="18"/>
       <c r="I14" s="23"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" s="14"/>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
@@ -924,12 +931,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I16" s="23"/>
     </row>
-    <row r="17" spans="7:9" ht="15.75">
+    <row r="17" spans="7:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G17" s="19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H17" s="20"/>
       <c r="I17" s="21">
@@ -947,19 +954,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="9" max="9" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>8</v>
       </c>
@@ -968,14 +975,14 @@
       <c r="D2" s="27"/>
       <c r="E2" s="27"/>
       <c r="G2" s="25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H2" s="26"/>
       <c r="I2" s="28"/>
     </row>
-    <row r="4" spans="1:9" ht="18.75">
+    <row r="4" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B4" s="33" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="33"/>
       <c r="D4" s="33"/>
@@ -984,7 +991,7 @@
       <c r="G4" s="33"/>
       <c r="H4" s="33"/>
     </row>
-    <row r="5" spans="1:9" ht="15.75">
+    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1007,10 +1014,10 @@
         <v>6</v>
       </c>
       <c r="I5" s="22" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
       <c r="C6" s="5">
         <v>1</v>
@@ -1032,7 +1039,7 @@
       </c>
       <c r="I6" s="23"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="10"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
@@ -1045,7 +1052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="7">
         <v>7</v>
       </c>
@@ -1069,7 +1076,7 @@
       </c>
       <c r="I8" s="23"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="12"/>
       <c r="C9" s="13"/>
       <c r="D9" s="12"/>
@@ -1082,7 +1089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" s="5">
         <v>14</v>
       </c>
@@ -1106,7 +1113,7 @@
       </c>
       <c r="I10" s="23"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
@@ -1119,7 +1126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" s="7">
         <v>21</v>
       </c>
@@ -1143,7 +1150,7 @@
       </c>
       <c r="I12" s="23"/>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" s="12"/>
       <c r="C13" s="13"/>
       <c r="D13" s="12"/>
@@ -1156,7 +1163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" s="5">
         <v>28</v>
       </c>
@@ -1174,7 +1181,7 @@
       <c r="H14" s="18"/>
       <c r="I14" s="23"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
@@ -1187,12 +1194,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I16" s="23"/>
     </row>
-    <row r="17" spans="7:9" ht="15.75">
+    <row r="17" spans="7:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G17" s="19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H17" s="20"/>
       <c r="I17" s="21">
@@ -1209,19 +1216,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="9" max="9" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>8</v>
       </c>
@@ -1230,14 +1237,14 @@
       <c r="D2" s="27"/>
       <c r="E2" s="27"/>
       <c r="G2" s="25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H2" s="26"/>
       <c r="I2" s="28"/>
     </row>
-    <row r="4" spans="1:9" ht="18.75">
+    <row r="4" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B4" s="33" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" s="33"/>
       <c r="D4" s="33"/>
@@ -1246,7 +1253,7 @@
       <c r="G4" s="33"/>
       <c r="H4" s="33"/>
     </row>
-    <row r="5" spans="1:9" ht="15.75">
+    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1269,10 +1276,10 @@
         <v>6</v>
       </c>
       <c r="I5" s="22" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
       <c r="C6" s="16"/>
       <c r="D6" s="16"/>
@@ -1288,7 +1295,7 @@
       </c>
       <c r="I6" s="23"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="10"/>
       <c r="C7" s="32"/>
       <c r="D7" s="32"/>
@@ -1301,7 +1308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="7">
         <v>4</v>
       </c>
@@ -1325,7 +1332,7 @@
       </c>
       <c r="I8" s="23"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="12"/>
       <c r="C9" s="13"/>
       <c r="D9" s="12"/>
@@ -1338,7 +1345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" s="5">
         <v>11</v>
       </c>
@@ -1362,7 +1369,7 @@
       </c>
       <c r="I10" s="23"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
@@ -1375,7 +1382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" s="7">
         <v>18</v>
       </c>
@@ -1399,7 +1406,7 @@
       </c>
       <c r="I12" s="23"/>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" s="12"/>
       <c r="C13" s="13"/>
       <c r="D13" s="12"/>
@@ -1412,7 +1419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" s="5">
         <v>25</v>
       </c>
@@ -1434,7 +1441,7 @@
       <c r="H14" s="31"/>
       <c r="I14" s="23"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
@@ -1447,12 +1454,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I16" s="23"/>
     </row>
-    <row r="17" spans="7:9" ht="15.75">
+    <row r="17" spans="7:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G17" s="19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H17" s="20"/>
       <c r="I17" s="21">
@@ -1469,19 +1476,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="9" max="9" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>8</v>
       </c>
@@ -1490,14 +1497,14 @@
       <c r="D2" s="27"/>
       <c r="E2" s="27"/>
       <c r="G2" s="25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H2" s="26"/>
       <c r="I2" s="28"/>
     </row>
-    <row r="4" spans="1:9" ht="18.75">
+    <row r="4" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B4" s="33" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="33"/>
       <c r="D4" s="33"/>
@@ -1506,7 +1513,7 @@
       <c r="G4" s="33"/>
       <c r="H4" s="33"/>
     </row>
-    <row r="5" spans="1:9" ht="15.75">
+    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1529,10 +1536,10 @@
         <v>6</v>
       </c>
       <c r="I5" s="22" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="5">
         <v>2</v>
       </c>
@@ -1556,7 +1563,7 @@
       </c>
       <c r="I6" s="23"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="29"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
@@ -1569,7 +1576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="7">
         <v>9</v>
       </c>
@@ -1593,7 +1600,7 @@
       </c>
       <c r="I8" s="23"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="12"/>
       <c r="C9" s="13"/>
       <c r="D9" s="12"/>
@@ -1606,7 +1613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" s="5">
         <v>16</v>
       </c>
@@ -1630,7 +1637,7 @@
       </c>
       <c r="I10" s="23"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
@@ -1643,7 +1650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" s="7">
         <v>23</v>
       </c>
@@ -1667,7 +1674,7 @@
       </c>
       <c r="I12" s="23"/>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" s="12"/>
       <c r="C13" s="13"/>
       <c r="D13" s="12"/>
@@ -1680,7 +1687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" s="5">
         <v>30</v>
       </c>
@@ -1694,7 +1701,7 @@
       <c r="H14" s="18"/>
       <c r="I14" s="23"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
       <c r="D15" s="15"/>
@@ -1707,12 +1714,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I16" s="23"/>
     </row>
-    <row r="17" spans="7:9" ht="15.75">
+    <row r="17" spans="7:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G17" s="19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H17" s="20"/>
       <c r="I17" s="21">

</xml_diff>

<commit_message>
Modificación de datos en la venta comisionable
</commit_message>
<xml_diff>
--- a/Documentos Adicionales/Ventas Adriana Jaramillo.xlsx
+++ b/Documentos Adicionales/Ventas Adriana Jaramillo.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="120" windowWidth="11655" windowHeight="6915"/>
@@ -12,7 +12,7 @@
     <sheet name="ABRIL" sheetId="3" r:id="rId3"/>
     <sheet name="MAYO" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -46,9 +46,6 @@
     <t>EJECUTIVO DE VENTAS:</t>
   </si>
   <si>
-    <t>Alma Yesenia Garcia Enriquez</t>
-  </si>
-  <si>
     <t>META COMISIONABLE:</t>
   </si>
   <si>
@@ -66,17 +63,20 @@
   <si>
     <t>MAYO</t>
   </si>
+  <si>
+    <t>Judith Adriana Jaramillo Chávez</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -347,13 +347,13 @@
     <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="44" fontId="2" fillId="10" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="2" fillId="12" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -366,6 +366,11 @@
       <color rgb="FFFFFF66"/>
     </mruColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -444,6 +449,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -478,6 +484,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -653,48 +660,48 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="9" max="9" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="25"/>
       <c r="C2" s="26" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D2" s="26"/>
       <c r="E2" s="26"/>
       <c r="G2" s="24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H2" s="25"/>
       <c r="I2" s="27">
         <v>43000</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="18.75">
-      <c r="B4" s="32" t="s">
+    <row r="4" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B4" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-    </row>
-    <row r="5" spans="1:9" ht="15.75">
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
@@ -717,10 +724,10 @@
         <v>6</v>
       </c>
       <c r="I5" s="21" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="4">
         <v>1</v>
       </c>
@@ -744,7 +751,7 @@
       </c>
       <c r="I6" s="22"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="9"/>
       <c r="C7" s="10">
         <v>0</v>
@@ -760,12 +767,12 @@
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="17"/>
-      <c r="I7" s="33">
+      <c r="I7" s="32">
         <f>B7+C7+D7+E7+F7</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="7">
         <v>8</v>
       </c>
@@ -787,9 +794,9 @@
       <c r="H8" s="6">
         <v>14</v>
       </c>
-      <c r="I8" s="34"/>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="I8" s="33"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="11">
         <v>825</v>
       </c>
@@ -807,12 +814,12 @@
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="17"/>
-      <c r="I9" s="33">
+      <c r="I9" s="32">
         <f>B9+C9+D9+E9+F9</f>
         <v>3300</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" s="5">
         <v>15</v>
       </c>
@@ -834,9 +841,9 @@
       <c r="H10" s="17">
         <v>21</v>
       </c>
-      <c r="I10" s="35"/>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="I10" s="34"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" s="13">
         <v>0</v>
       </c>
@@ -854,12 +861,12 @@
       </c>
       <c r="G11" s="6"/>
       <c r="H11" s="17"/>
-      <c r="I11" s="33">
+      <c r="I11" s="32">
         <f>B11+C11+D11+E11+F11</f>
         <v>6915</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" s="7">
         <v>22</v>
       </c>
@@ -881,9 +888,9 @@
       <c r="H12" s="17">
         <v>28</v>
       </c>
-      <c r="I12" s="35"/>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="I12" s="34"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" s="11">
         <v>825</v>
       </c>
@@ -901,12 +908,12 @@
       </c>
       <c r="G13" s="6"/>
       <c r="H13" s="17"/>
-      <c r="I13" s="33">
+      <c r="I13" s="32">
         <f>B13+C13+D13+E13+F13</f>
         <v>1485</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" s="5">
         <v>29</v>
       </c>
@@ -916,32 +923,34 @@
       <c r="F14" s="15"/>
       <c r="G14" s="6"/>
       <c r="H14" s="17"/>
-      <c r="I14" s="35"/>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="B15" s="13"/>
+      <c r="I14" s="34"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="13">
+        <v>297</v>
+      </c>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
       <c r="E15" s="14"/>
       <c r="F15" s="14"/>
       <c r="G15" s="6"/>
       <c r="H15" s="17"/>
-      <c r="I15" s="33">
+      <c r="I15" s="32">
         <f>B15</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="I16" s="35"/>
-    </row>
-    <row r="17" spans="7:9" ht="15.75">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I16" s="34"/>
+    </row>
+    <row r="17" spans="7:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G17" s="18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H17" s="19"/>
-      <c r="I17" s="36">
+      <c r="I17" s="35">
         <f>I7+I9+I11+I13+I15</f>
-        <v>11700</v>
+        <v>11997</v>
       </c>
     </row>
   </sheetData>
@@ -954,19 +963,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="9" max="9" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>8</v>
       </c>
@@ -975,23 +984,23 @@
       <c r="D2" s="26"/>
       <c r="E2" s="26"/>
       <c r="G2" s="24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H2" s="25"/>
       <c r="I2" s="27"/>
     </row>
-    <row r="4" spans="1:9" ht="18.75">
-      <c r="B4" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-    </row>
-    <row r="5" spans="1:9" ht="15.75">
+    <row r="4" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B4" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1014,10 +1023,10 @@
         <v>6</v>
       </c>
       <c r="I5" s="21" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
       <c r="C6" s="5">
         <v>1</v>
@@ -1039,7 +1048,7 @@
       </c>
       <c r="I6" s="22"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="9"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -1052,7 +1061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="7">
         <v>7</v>
       </c>
@@ -1076,7 +1085,7 @@
       </c>
       <c r="I8" s="22"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="11"/>
       <c r="C9" s="12"/>
       <c r="D9" s="11"/>
@@ -1089,7 +1098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" s="5">
         <v>14</v>
       </c>
@@ -1113,7 +1122,7 @@
       </c>
       <c r="I10" s="22"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" s="13"/>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
@@ -1126,7 +1135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" s="7">
         <v>21</v>
       </c>
@@ -1150,7 +1159,7 @@
       </c>
       <c r="I12" s="22"/>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" s="11"/>
       <c r="C13" s="12"/>
       <c r="D13" s="11"/>
@@ -1163,7 +1172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" s="5">
         <v>28</v>
       </c>
@@ -1181,7 +1190,7 @@
       <c r="H14" s="17"/>
       <c r="I14" s="22"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" s="13"/>
       <c r="C15" s="13"/>
       <c r="D15" s="13"/>
@@ -1194,12 +1203,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I16" s="22"/>
     </row>
-    <row r="17" spans="7:9" ht="15.75">
+    <row r="17" spans="7:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G17" s="18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H17" s="19"/>
       <c r="I17" s="20">
@@ -1216,19 +1225,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="9" max="9" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>8</v>
       </c>
@@ -1237,23 +1246,23 @@
       <c r="D2" s="26"/>
       <c r="E2" s="26"/>
       <c r="G2" s="24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H2" s="25"/>
       <c r="I2" s="27"/>
     </row>
-    <row r="4" spans="1:9" ht="18.75">
-      <c r="B4" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-    </row>
-    <row r="5" spans="1:9" ht="15.75">
+    <row r="4" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B4" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1276,10 +1285,10 @@
         <v>6</v>
       </c>
       <c r="I5" s="21" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
       <c r="C6" s="15"/>
       <c r="D6" s="15"/>
@@ -1295,7 +1304,7 @@
       </c>
       <c r="I6" s="22"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="9"/>
       <c r="C7" s="31"/>
       <c r="D7" s="31"/>
@@ -1308,7 +1317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="7">
         <v>4</v>
       </c>
@@ -1332,7 +1341,7 @@
       </c>
       <c r="I8" s="22"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="11"/>
       <c r="C9" s="12"/>
       <c r="D9" s="11"/>
@@ -1345,7 +1354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" s="5">
         <v>11</v>
       </c>
@@ -1369,7 +1378,7 @@
       </c>
       <c r="I10" s="22"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" s="13"/>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
@@ -1382,7 +1391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" s="7">
         <v>18</v>
       </c>
@@ -1406,7 +1415,7 @@
       </c>
       <c r="I12" s="22"/>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" s="11"/>
       <c r="C13" s="12"/>
       <c r="D13" s="11"/>
@@ -1419,7 +1428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" s="5">
         <v>25</v>
       </c>
@@ -1441,7 +1450,7 @@
       <c r="H14" s="30"/>
       <c r="I14" s="22"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" s="13"/>
       <c r="C15" s="13"/>
       <c r="D15" s="13"/>
@@ -1454,12 +1463,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I16" s="22"/>
     </row>
-    <row r="17" spans="7:9" ht="15.75">
+    <row r="17" spans="7:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G17" s="18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H17" s="19"/>
       <c r="I17" s="20">
@@ -1476,19 +1485,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="9" max="9" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>8</v>
       </c>
@@ -1497,23 +1506,23 @@
       <c r="D2" s="26"/>
       <c r="E2" s="26"/>
       <c r="G2" s="24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H2" s="25"/>
       <c r="I2" s="27"/>
     </row>
-    <row r="4" spans="1:9" ht="18.75">
-      <c r="B4" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-    </row>
-    <row r="5" spans="1:9" ht="15.75">
+    <row r="4" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B4" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1536,10 +1545,10 @@
         <v>6</v>
       </c>
       <c r="I5" s="21" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="5">
         <v>2</v>
       </c>
@@ -1563,7 +1572,7 @@
       </c>
       <c r="I6" s="22"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="28"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -1576,7 +1585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="7">
         <v>9</v>
       </c>
@@ -1600,7 +1609,7 @@
       </c>
       <c r="I8" s="22"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="11"/>
       <c r="C9" s="12"/>
       <c r="D9" s="11"/>
@@ -1613,7 +1622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" s="5">
         <v>16</v>
       </c>
@@ -1637,7 +1646,7 @@
       </c>
       <c r="I10" s="22"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" s="13"/>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
@@ -1650,7 +1659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" s="7">
         <v>23</v>
       </c>
@@ -1674,7 +1683,7 @@
       </c>
       <c r="I12" s="22"/>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" s="11"/>
       <c r="C13" s="12"/>
       <c r="D13" s="11"/>
@@ -1687,7 +1696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" s="5">
         <v>30</v>
       </c>
@@ -1701,7 +1710,7 @@
       <c r="H14" s="17"/>
       <c r="I14" s="22"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" s="13"/>
       <c r="C15" s="13"/>
       <c r="D15" s="14"/>
@@ -1714,12 +1723,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I16" s="22"/>
     </row>
-    <row r="17" spans="7:9" ht="15.75">
+    <row r="17" spans="7:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G17" s="18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H17" s="19"/>
       <c r="I17" s="20">

</xml_diff>

<commit_message>
Actualización de datos de ventas
</commit_message>
<xml_diff>
--- a/Documentos Adicionales/Ventas Adriana Jaramillo.xlsx
+++ b/Documentos Adicionales/Ventas Adriana Jaramillo.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="120" windowWidth="11655" windowHeight="6915"/>
@@ -12,7 +12,7 @@
     <sheet name="ABRIL" sheetId="3" r:id="rId3"/>
     <sheet name="MAYO" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -91,13 +91,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -310,7 +310,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -421,11 +421,12 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentual" xfId="2" builtinId="5"/>
+    <cellStyle name="Porcentaje" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -517,6 +518,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -551,6 +553,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -726,21 +729,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:N17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="9" max="9" width="17.42578125" customWidth="1"/>
     <col min="10" max="10" width="18.7109375" customWidth="1"/>
     <col min="11" max="11" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>8</v>
       </c>
@@ -758,7 +761,7 @@
         <v>41000</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="18.75">
+    <row r="4" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B4" s="50" t="s">
         <v>12</v>
       </c>
@@ -769,7 +772,7 @@
       <c r="G4" s="50"/>
       <c r="H4" s="50"/>
     </row>
-    <row r="5" spans="1:14" ht="15.75">
+    <row r="5" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
@@ -801,7 +804,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>9</v>
       </c>
@@ -828,7 +831,7 @@
       <c r="J6" s="37"/>
       <c r="K6" s="44"/>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B7" s="9"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -848,7 +851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>10</v>
       </c>
@@ -877,7 +880,7 @@
       <c r="J8" s="39"/>
       <c r="K8" s="44"/>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B9" s="11"/>
       <c r="C9" s="12">
         <v>825</v>
@@ -903,7 +906,7 @@
         <v>19.341463414634145</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>11</v>
       </c>
@@ -932,7 +935,7 @@
       <c r="J10" s="39"/>
       <c r="K10" s="44"/>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B11" s="13"/>
       <c r="C11" s="13"/>
       <c r="D11" s="13">
@@ -956,7 +959,7 @@
         <v>16.865853658536587</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>12</v>
       </c>
@@ -985,7 +988,7 @@
       <c r="J12" s="39"/>
       <c r="K12" s="44"/>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B13" s="14"/>
       <c r="C13" s="12">
         <v>1017</v>
@@ -1007,7 +1010,7 @@
         <v>17.858231707317074</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1030,27 +1033,31 @@
       <c r="J14" s="39"/>
       <c r="K14" s="44"/>
     </row>
-    <row r="15" spans="1:14">
-      <c r="B15" s="13"/>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B15" s="13">
+        <v>2808.5</v>
+      </c>
       <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
+      <c r="D15" s="13">
+        <v>297</v>
+      </c>
       <c r="E15" s="13"/>
       <c r="F15" s="14"/>
       <c r="G15" s="6"/>
       <c r="H15" s="17"/>
       <c r="I15" s="49">
         <f>B15+C15+D15+E15</f>
-        <v>0</v>
+        <v>3105.5</v>
       </c>
       <c r="J15" s="38">
         <v>8200</v>
       </c>
       <c r="K15" s="45">
         <f>((I15+I13+I11+I9+I7)*100)/(J11+J13+J15+J9+J7)</f>
-        <v>14.286585365853659</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14">
+        <v>21.860975609756096</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I16" s="22"/>
       <c r="J16" s="39"/>
       <c r="K16" s="46"/>
@@ -1060,14 +1067,14 @@
       <c r="M16" s="48"/>
       <c r="N16" s="48"/>
     </row>
-    <row r="17" spans="7:14" ht="15.75">
+    <row r="17" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G17" s="18" t="s">
         <v>11</v>
       </c>
       <c r="H17" s="19"/>
       <c r="I17" s="20">
         <f>I7+I9+I11+I13+I15</f>
-        <v>5857.5</v>
+        <v>8963</v>
       </c>
       <c r="J17" s="40">
         <f>J7+J9+J11+J13+J15</f>
@@ -1076,10 +1083,13 @@
       <c r="K17" s="46"/>
       <c r="L17" s="51">
         <f>I17*100/J17</f>
-        <v>14.286585365853659</v>
+        <v>21.860975609756096</v>
       </c>
       <c r="M17" s="52"/>
       <c r="N17" s="53"/>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B18" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1091,19 +1101,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="9" max="9" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>8</v>
       </c>
@@ -1121,7 +1131,7 @@
         <v>43000</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="18.75">
+    <row r="4" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B4" s="50" t="s">
         <v>7</v>
       </c>
@@ -1132,7 +1142,7 @@
       <c r="G4" s="50"/>
       <c r="H4" s="50"/>
     </row>
-    <row r="5" spans="1:9" ht="15.75">
+    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1158,7 +1168,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1185,7 +1195,7 @@
       </c>
       <c r="I6" s="22"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="9"/>
       <c r="C7" s="10">
         <v>0</v>
@@ -1206,7 +1216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1233,7 +1243,7 @@
       </c>
       <c r="I8" s="33"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="11">
         <v>825</v>
       </c>
@@ -1256,7 +1266,7 @@
         <v>3300</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
@@ -1283,7 +1293,7 @@
       </c>
       <c r="I10" s="34"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" s="13">
         <v>0</v>
       </c>
@@ -1306,7 +1316,7 @@
         <v>6915</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
@@ -1333,7 +1343,7 @@
       </c>
       <c r="I12" s="34"/>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" s="11">
         <v>825</v>
       </c>
@@ -1356,7 +1366,7 @@
         <v>1485</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>9</v>
       </c>
@@ -1371,7 +1381,7 @@
       <c r="H14" s="17"/>
       <c r="I14" s="34"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" s="13">
         <v>297</v>
       </c>
@@ -1386,10 +1396,10 @@
         <v>297</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I16" s="34"/>
     </row>
-    <row r="17" spans="7:10" ht="15.75">
+    <row r="17" spans="7:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G17" s="18" t="s">
         <v>11</v>
       </c>
@@ -1412,19 +1422,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="9" max="9" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>8</v>
       </c>
@@ -1438,7 +1448,7 @@
       <c r="H2" s="25"/>
       <c r="I2" s="27"/>
     </row>
-    <row r="4" spans="1:9" ht="18.75">
+    <row r="4" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B4" s="50" t="s">
         <v>13</v>
       </c>
@@ -1449,7 +1459,7 @@
       <c r="G4" s="50"/>
       <c r="H4" s="50"/>
     </row>
-    <row r="5" spans="1:9" ht="15.75">
+    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1475,7 +1485,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
       <c r="C6" s="15"/>
       <c r="D6" s="15"/>
@@ -1491,7 +1501,7 @@
       </c>
       <c r="I6" s="22"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="9"/>
       <c r="C7" s="31"/>
       <c r="D7" s="31"/>
@@ -1504,7 +1514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="7">
         <v>4</v>
       </c>
@@ -1528,7 +1538,7 @@
       </c>
       <c r="I8" s="22"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="11"/>
       <c r="C9" s="12"/>
       <c r="D9" s="11"/>
@@ -1541,7 +1551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" s="5">
         <v>11</v>
       </c>
@@ -1565,7 +1575,7 @@
       </c>
       <c r="I10" s="22"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" s="13"/>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
@@ -1578,7 +1588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" s="7">
         <v>18</v>
       </c>
@@ -1602,7 +1612,7 @@
       </c>
       <c r="I12" s="22"/>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" s="11"/>
       <c r="C13" s="12"/>
       <c r="D13" s="11"/>
@@ -1615,7 +1625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" s="5">
         <v>25</v>
       </c>
@@ -1637,7 +1647,7 @@
       <c r="H14" s="30"/>
       <c r="I14" s="22"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" s="13"/>
       <c r="C15" s="13"/>
       <c r="D15" s="13"/>
@@ -1650,10 +1660,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I16" s="22"/>
     </row>
-    <row r="17" spans="7:9" ht="15.75">
+    <row r="17" spans="7:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G17" s="18" t="s">
         <v>11</v>
       </c>
@@ -1672,19 +1682,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="9" max="9" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>8</v>
       </c>
@@ -1698,7 +1708,7 @@
       <c r="H2" s="25"/>
       <c r="I2" s="27"/>
     </row>
-    <row r="4" spans="1:9" ht="18.75">
+    <row r="4" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B4" s="50" t="s">
         <v>14</v>
       </c>
@@ -1709,7 +1719,7 @@
       <c r="G4" s="50"/>
       <c r="H4" s="50"/>
     </row>
-    <row r="5" spans="1:9" ht="15.75">
+    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1735,7 +1745,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="5">
         <v>2</v>
       </c>
@@ -1759,7 +1769,7 @@
       </c>
       <c r="I6" s="22"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="28"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -1772,7 +1782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="7">
         <v>9</v>
       </c>
@@ -1796,7 +1806,7 @@
       </c>
       <c r="I8" s="22"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="11"/>
       <c r="C9" s="12"/>
       <c r="D9" s="11"/>
@@ -1809,7 +1819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" s="5">
         <v>16</v>
       </c>
@@ -1833,7 +1843,7 @@
       </c>
       <c r="I10" s="22"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" s="13"/>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
@@ -1846,7 +1856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" s="7">
         <v>23</v>
       </c>
@@ -1870,7 +1880,7 @@
       </c>
       <c r="I12" s="22"/>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" s="11"/>
       <c r="C13" s="12"/>
       <c r="D13" s="11"/>
@@ -1883,7 +1893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" s="5">
         <v>30</v>
       </c>
@@ -1897,7 +1907,7 @@
       <c r="H14" s="17"/>
       <c r="I14" s="22"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" s="13"/>
       <c r="C15" s="13"/>
       <c r="D15" s="14"/>
@@ -1910,10 +1920,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I16" s="22"/>
     </row>
-    <row r="17" spans="7:9" ht="15.75">
+    <row r="17" spans="7:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G17" s="18" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Actualización de ventas comisionadas
</commit_message>
<xml_diff>
--- a/Documentos Adicionales/Ventas Adriana Jaramillo.xlsx
+++ b/Documentos Adicionales/Ventas Adriana Jaramillo.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="11655" windowHeight="6915"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="11655" windowHeight="6915" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="MARZO" sheetId="2" r:id="rId1"/>
-    <sheet name="FEBRERO" sheetId="1" r:id="rId2"/>
+    <sheet name="FEBRERO" sheetId="1" r:id="rId1"/>
+    <sheet name="MARZO" sheetId="2" r:id="rId2"/>
     <sheet name="ABRIL" sheetId="3" r:id="rId3"/>
     <sheet name="MAYO" sheetId="4" r:id="rId4"/>
   </sheets>
@@ -730,10 +730,331 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:J17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="9" width="18.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="25"/>
+      <c r="C2" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="G2" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="25"/>
+      <c r="I2" s="27">
+        <v>43000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B4" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51"/>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" s="21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4">
+        <v>1</v>
+      </c>
+      <c r="C6" s="5">
+        <v>2</v>
+      </c>
+      <c r="D6" s="5">
+        <v>3</v>
+      </c>
+      <c r="E6" s="5">
+        <v>4</v>
+      </c>
+      <c r="F6" s="5">
+        <v>5</v>
+      </c>
+      <c r="G6" s="6">
+        <v>6</v>
+      </c>
+      <c r="H6" s="17">
+        <v>7</v>
+      </c>
+      <c r="I6" s="22"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="9"/>
+      <c r="C7" s="10">
+        <v>0</v>
+      </c>
+      <c r="D7" s="10">
+        <v>0</v>
+      </c>
+      <c r="E7" s="10">
+        <v>0</v>
+      </c>
+      <c r="F7" s="10">
+        <v>0</v>
+      </c>
+      <c r="G7" s="6"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="32">
+        <f>B7+C7+D7+E7+F7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="7">
+        <v>8</v>
+      </c>
+      <c r="C8" s="8">
+        <v>9</v>
+      </c>
+      <c r="D8" s="7">
+        <v>10</v>
+      </c>
+      <c r="E8" s="8">
+        <v>11</v>
+      </c>
+      <c r="F8" s="7">
+        <v>12</v>
+      </c>
+      <c r="G8" s="6">
+        <v>13</v>
+      </c>
+      <c r="H8" s="6">
+        <v>14</v>
+      </c>
+      <c r="I8" s="33"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="11">
+        <v>825</v>
+      </c>
+      <c r="C9" s="12">
+        <v>825</v>
+      </c>
+      <c r="D9" s="11">
+        <v>0</v>
+      </c>
+      <c r="E9" s="12">
+        <v>1650</v>
+      </c>
+      <c r="F9" s="11">
+        <v>0</v>
+      </c>
+      <c r="G9" s="6"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="32">
+        <f>B9+C9+D9+E9+F9</f>
+        <v>3300</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10" s="5">
+        <v>15</v>
+      </c>
+      <c r="C10" s="5">
+        <v>16</v>
+      </c>
+      <c r="D10" s="5">
+        <v>17</v>
+      </c>
+      <c r="E10" s="5">
+        <v>18</v>
+      </c>
+      <c r="F10" s="5">
+        <v>19</v>
+      </c>
+      <c r="G10" s="6">
+        <v>20</v>
+      </c>
+      <c r="H10" s="17">
+        <v>21</v>
+      </c>
+      <c r="I10" s="34"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="13">
+        <v>0</v>
+      </c>
+      <c r="C11" s="13">
+        <v>709.5</v>
+      </c>
+      <c r="D11" s="13">
+        <v>0</v>
+      </c>
+      <c r="E11" s="13">
+        <v>5008.5</v>
+      </c>
+      <c r="F11" s="13">
+        <v>1197</v>
+      </c>
+      <c r="G11" s="6"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="32">
+        <f>B11+C11+D11+E11+F11</f>
+        <v>6915</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12" s="7">
+        <v>22</v>
+      </c>
+      <c r="C12" s="8">
+        <v>23</v>
+      </c>
+      <c r="D12" s="7">
+        <v>24</v>
+      </c>
+      <c r="E12" s="8">
+        <v>25</v>
+      </c>
+      <c r="F12" s="7">
+        <v>26</v>
+      </c>
+      <c r="G12" s="6">
+        <v>27</v>
+      </c>
+      <c r="H12" s="17">
+        <v>28</v>
+      </c>
+      <c r="I12" s="34"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="11">
+        <v>825</v>
+      </c>
+      <c r="C13" s="12">
+        <v>0</v>
+      </c>
+      <c r="D13" s="11">
+        <v>412.5</v>
+      </c>
+      <c r="E13" s="12">
+        <v>247.5</v>
+      </c>
+      <c r="F13" s="11">
+        <v>0</v>
+      </c>
+      <c r="G13" s="6"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="32">
+        <f>B13+C13+D13+E13+F13</f>
+        <v>1485</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>9</v>
+      </c>
+      <c r="B14" s="5">
+        <v>29</v>
+      </c>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="34"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="13">
+        <v>297</v>
+      </c>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="32">
+        <f>B15</f>
+        <v>297</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I16" s="34"/>
+    </row>
+    <row r="17" spans="7:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G17" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" s="19"/>
+      <c r="I17" s="35">
+        <f>I7+I9+I11+I13+I15</f>
+        <v>11997</v>
+      </c>
+      <c r="J17">
+        <v>27.9</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B4:H4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1026,7 +1347,9 @@
       <c r="E14" s="5">
         <v>31</v>
       </c>
-      <c r="F14" s="15"/>
+      <c r="F14" s="15">
+        <v>1</v>
+      </c>
       <c r="G14" s="6"/>
       <c r="H14" s="17"/>
       <c r="I14" s="22"/>
@@ -1044,19 +1367,21 @@
       <c r="E15" s="13">
         <v>1284</v>
       </c>
-      <c r="F15" s="14"/>
+      <c r="F15" s="14">
+        <v>2034</v>
+      </c>
       <c r="G15" s="6"/>
       <c r="H15" s="17"/>
       <c r="I15" s="49">
-        <f>B15+C15+D15+E15</f>
-        <v>4389.5</v>
+        <f>B15+C15+D15+E15+F15</f>
+        <v>6423.5</v>
       </c>
       <c r="J15" s="38">
         <v>8200</v>
       </c>
       <c r="K15" s="45">
         <f>((I15+I13+I11+I9+I7)*100)/(J11+J13+J15+J9+J7)</f>
-        <v>24.992682926829268</v>
+        <v>29.953658536585365</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -1076,7 +1401,7 @@
       <c r="H17" s="19"/>
       <c r="I17" s="20">
         <f>I7+I9+I11+I13+I15</f>
-        <v>10247</v>
+        <v>12281</v>
       </c>
       <c r="J17" s="40">
         <f>J7+J9+J11+J13+J15</f>
@@ -1085,7 +1410,7 @@
       <c r="K17" s="46"/>
       <c r="L17" s="52">
         <f>I17*100/J17</f>
-        <v>24.992682926829268</v>
+        <v>29.953658536585365</v>
       </c>
       <c r="M17" s="53"/>
       <c r="N17" s="54"/>
@@ -1099,327 +1424,6 @@
     <mergeCell ref="L17:N17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="9" max="9" width="18.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="G2" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="25"/>
-      <c r="I2" s="27">
-        <v>43000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B4" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="51"/>
-    </row>
-    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H5" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="I5" s="21" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4">
-        <v>1</v>
-      </c>
-      <c r="C6" s="5">
-        <v>2</v>
-      </c>
-      <c r="D6" s="5">
-        <v>3</v>
-      </c>
-      <c r="E6" s="5">
-        <v>4</v>
-      </c>
-      <c r="F6" s="5">
-        <v>5</v>
-      </c>
-      <c r="G6" s="6">
-        <v>6</v>
-      </c>
-      <c r="H6" s="17">
-        <v>7</v>
-      </c>
-      <c r="I6" s="22"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="9"/>
-      <c r="C7" s="10">
-        <v>0</v>
-      </c>
-      <c r="D7" s="10">
-        <v>0</v>
-      </c>
-      <c r="E7" s="10">
-        <v>0</v>
-      </c>
-      <c r="F7" s="10">
-        <v>0</v>
-      </c>
-      <c r="G7" s="6"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="32">
-        <f>B7+C7+D7+E7+F7</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" s="7">
-        <v>8</v>
-      </c>
-      <c r="C8" s="8">
-        <v>9</v>
-      </c>
-      <c r="D8" s="7">
-        <v>10</v>
-      </c>
-      <c r="E8" s="8">
-        <v>11</v>
-      </c>
-      <c r="F8" s="7">
-        <v>12</v>
-      </c>
-      <c r="G8" s="6">
-        <v>13</v>
-      </c>
-      <c r="H8" s="6">
-        <v>14</v>
-      </c>
-      <c r="I8" s="33"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="11">
-        <v>825</v>
-      </c>
-      <c r="C9" s="12">
-        <v>825</v>
-      </c>
-      <c r="D9" s="11">
-        <v>0</v>
-      </c>
-      <c r="E9" s="12">
-        <v>1650</v>
-      </c>
-      <c r="F9" s="11">
-        <v>0</v>
-      </c>
-      <c r="G9" s="6"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="32">
-        <f>B9+C9+D9+E9+F9</f>
-        <v>3300</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>7</v>
-      </c>
-      <c r="B10" s="5">
-        <v>15</v>
-      </c>
-      <c r="C10" s="5">
-        <v>16</v>
-      </c>
-      <c r="D10" s="5">
-        <v>17</v>
-      </c>
-      <c r="E10" s="5">
-        <v>18</v>
-      </c>
-      <c r="F10" s="5">
-        <v>19</v>
-      </c>
-      <c r="G10" s="6">
-        <v>20</v>
-      </c>
-      <c r="H10" s="17">
-        <v>21</v>
-      </c>
-      <c r="I10" s="34"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="13">
-        <v>0</v>
-      </c>
-      <c r="C11" s="13">
-        <v>709.5</v>
-      </c>
-      <c r="D11" s="13">
-        <v>0</v>
-      </c>
-      <c r="E11" s="13">
-        <v>5008.5</v>
-      </c>
-      <c r="F11" s="13">
-        <v>1197</v>
-      </c>
-      <c r="G11" s="6"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="32">
-        <f>B11+C11+D11+E11+F11</f>
-        <v>6915</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>8</v>
-      </c>
-      <c r="B12" s="7">
-        <v>22</v>
-      </c>
-      <c r="C12" s="8">
-        <v>23</v>
-      </c>
-      <c r="D12" s="7">
-        <v>24</v>
-      </c>
-      <c r="E12" s="8">
-        <v>25</v>
-      </c>
-      <c r="F12" s="7">
-        <v>26</v>
-      </c>
-      <c r="G12" s="6">
-        <v>27</v>
-      </c>
-      <c r="H12" s="17">
-        <v>28</v>
-      </c>
-      <c r="I12" s="34"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="11">
-        <v>825</v>
-      </c>
-      <c r="C13" s="12">
-        <v>0</v>
-      </c>
-      <c r="D13" s="11">
-        <v>412.5</v>
-      </c>
-      <c r="E13" s="12">
-        <v>247.5</v>
-      </c>
-      <c r="F13" s="11">
-        <v>0</v>
-      </c>
-      <c r="G13" s="6"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="32">
-        <f>B13+C13+D13+E13+F13</f>
-        <v>1485</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>9</v>
-      </c>
-      <c r="B14" s="5">
-        <v>29</v>
-      </c>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="34"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="13">
-        <v>297</v>
-      </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="32">
-        <f>B15</f>
-        <v>297</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I16" s="34"/>
-    </row>
-    <row r="17" spans="7:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G17" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="H17" s="19"/>
-      <c r="I17" s="35">
-        <f>I7+I9+I11+I13+I15</f>
-        <v>11997</v>
-      </c>
-      <c r="J17">
-        <v>27.9</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B4:H4"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Actualización de venta comisionable
</commit_message>
<xml_diff>
--- a/Documentos Adicionales/Ventas Adriana Jaramillo.xlsx
+++ b/Documentos Adicionales/Ventas Adriana Jaramillo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="11655" windowHeight="6915" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="180" windowWidth="11655" windowHeight="6855" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="FEBRERO" sheetId="1" r:id="rId1"/>
@@ -1053,8 +1053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1431,8 +1431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1512,12 +1512,14 @@
       <c r="C7" s="31"/>
       <c r="D7" s="31"/>
       <c r="E7" s="31"/>
-      <c r="F7" s="10"/>
+      <c r="F7" s="10">
+        <v>2034</v>
+      </c>
       <c r="G7" s="29"/>
       <c r="H7" s="30"/>
       <c r="I7" s="23">
         <f>B7+C7+D7+E7+F7</f>
-        <v>0</v>
+        <v>2034</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1545,8 +1547,12 @@
       <c r="I8" s="22"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="11"/>
-      <c r="C9" s="12"/>
+      <c r="B9" s="11">
+        <v>1429.5</v>
+      </c>
+      <c r="C9" s="12">
+        <v>1617</v>
+      </c>
       <c r="D9" s="11"/>
       <c r="E9" s="12"/>
       <c r="F9" s="11"/>
@@ -1554,7 +1560,7 @@
       <c r="H9" s="30"/>
       <c r="I9" s="23">
         <f>B9+C9+D9+E9+F9</f>
-        <v>0</v>
+        <v>3046.5</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1676,7 +1682,7 @@
       <c r="H17" s="19"/>
       <c r="I17" s="20">
         <f>I7+I9+I11+I13+I15</f>
-        <v>0</v>
+        <v>5080.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>